<commit_message>
updated cover sheet template. started explore NB to update the save rtpa outputs function. mainly, changes to the excel writer portion so it only writes data related to the RTPA, not the entire dataset.
</commit_message>
<xml_diff>
--- a/ntd/cover_sheet_template.xlsx
+++ b/ntd/cover_sheet_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://caltrans-my.sharepoint.com/personal/christian_suyat_dot_ca_gov/Documents/HomeDirectory/2023-08-04_Division of Data and Digital Services/2023-12-12_897_bus_procurement_cost_and_award/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s145252\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="71" documentId="8_{749355A0-8D2F-4F2F-8F27-41070AD47DC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B47B57B7-4307-4F12-BE1F-86BF084516C7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5257C666-F6B3-4BFF-BE36-E791CBBEDE6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28950" yWindow="2520" windowWidth="14790" windowHeight="11325" xr2:uid="{E7B44C33-9732-4AC6-B6B9-D7189BBEABAD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{E7B44C33-9732-4AC6-B6B9-D7189BBEABAD}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="1" r:id="rId1"/>
@@ -36,13 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="102">
-  <si>
-    <t>NTD Monthly Ridership by RTPA</t>
-  </si>
-  <si>
-    <t>Provide CalSTA with NTD Monthly Ridership by each regional transportation planning authority (RTPA).</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="108">
   <si>
     <t>This report shows general ridership trends by transit agency, mode, and type of service. Reported unlinked passenger trips are reported, as well as the change from the prior year. For example, July 2023’s change would be the change in July 2023’s reported values against July 2022’s reported values.</t>
   </si>
@@ -50,9 +44,6 @@
     <t xml:space="preserve"> Purchased Transportation - Taxi</t>
   </si>
   <si>
-    <t>NTD Modes</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Commuter Bus</t>
   </si>
   <si>
@@ -104,9 +95,6 @@
     <t xml:space="preserve"> Purchased Transportation - Transportation Network Company</t>
   </si>
   <si>
-    <t>Data Dictionary</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
@@ -248,21 +236,9 @@
     <t>TX</t>
   </si>
   <si>
-    <t>NTD Type of Service (TOS)</t>
-  </si>
-  <si>
     <t>RTPA Ridership Data</t>
   </si>
   <si>
-    <t>The processed data used to populate the Monthly NTD Ridership Portfolio charts and graphs for reach RTPA</t>
-  </si>
-  <si>
-    <t>Workbook Tabs</t>
-  </si>
-  <si>
-    <t>Column Names</t>
-  </si>
-  <si>
     <t>Definition</t>
   </si>
   <si>
@@ -342,6 +318,48 @@
   </si>
   <si>
     <t>Dt</t>
+  </si>
+  <si>
+    <t>**NTD Monthly Ridership by RTPA**</t>
+  </si>
+  <si>
+    <t>**Workbook Tabs**</t>
+  </si>
+  <si>
+    <t>**Data Dictionary**</t>
+  </si>
+  <si>
+    <t>**NTD Modes**</t>
+  </si>
+  <si>
+    <t>**NTD Type of Service (TOS)**</t>
+  </si>
+  <si>
+    <t>**Column Names**</t>
+  </si>
+  <si>
+    <t>Aggregated by Agency</t>
+  </si>
+  <si>
+    <t>Aggregated by Mode</t>
+  </si>
+  <si>
+    <t>Aggregate by TOS</t>
+  </si>
+  <si>
+    <t>Provide CalSTA and RTPAs with NTD Monthly Ridership</t>
+  </si>
+  <si>
+    <t>The processed ridership data used to populate the Monthly NTD Ridership Portfolio charts and graphs for reach RTPA</t>
+  </si>
+  <si>
+    <t>The processed data, aggregated by individual transit agency, by year and month</t>
+  </si>
+  <si>
+    <t>The processed data, aggregated by NTD Mode (see data dictionary below), by year and month</t>
+  </si>
+  <si>
+    <t>The processed data, aggregated by NTD Type of Service (see data dictionary below), by year and month</t>
   </si>
 </sst>
 </file>
@@ -391,27 +409,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -436,7 +439,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -753,11 +756,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4A63280-4CAE-42D6-B3D9-7BBD49D66E76}">
-  <dimension ref="A1:F64"/>
+  <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -768,18 +769,18 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>0</v>
+        <v>94</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -788,10 +789,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -812,7 +813,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>73</v>
+        <v>95</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
@@ -821,10 +822,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>72</v>
+        <v>104</v>
       </c>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
@@ -832,334 +833,340 @@
       <c r="F7" s="8"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>105</v>
+      </c>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
     </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>22</v>
+      <c r="A10" s="5" t="s">
+        <v>102</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>75</v>
+        <v>107</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>5</v>
+      <c r="A13" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>6</v>
+      <c r="A15" s="3" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>19</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>20</v>
+      <c r="A32" s="3" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B37" s="2"/>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>28</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="B39" s="2" t="s">
+      <c r="A39" s="3" t="s">
         <v>99</v>
       </c>
+      <c r="B39" s="2"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
-        <v>101</v>
+        <v>76</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>100</v>
+        <v>29</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
-        <v>44</v>
+        <v>93</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>43</v>
+        <v>92</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
-        <v>23</v>
+        <v>73</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
-        <v>89</v>
+        <v>40</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
-        <v>90</v>
+        <v>20</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
-        <v>92</v>
+        <v>19</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>27</v>
@@ -1167,61 +1174,80 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
-        <v>24</v>
+        <v>90</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="9" t="s">
-        <v>94</v>
+        <v>69</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>37</v>
+        <v>91</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
-        <v>96</v>
+        <v>68</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>36</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A40:B66">
+    <sortCondition ref="A40:A66"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>